<commit_message>
adding utility to figure
</commit_message>
<xml_diff>
--- a/inst/extdata/byhand_distribution-cheat-sheet3.xlsx
+++ b/inst/extdata/byhand_distribution-cheat-sheet3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\au757887\PC_documents\_git-it\PESTO\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0DDF28A-0E55-41BA-AF40-4A4D0F733859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8839F646-1457-443F-A236-D40F5DBEC12F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{AFCE3043-D670-4FEA-ACB5-43895439CF13}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AFCE3043-D670-4FEA-ACB5-43895439CF13}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
   <si>
     <t>L</t>
   </si>
@@ -62,22 +62,25 @@
     <t>Use R simulations of the beta-distribution to figure out how to distribute it amonst the other bins</t>
   </si>
   <si>
-    <t>very high value</t>
-  </si>
-  <si>
-    <t>high value</t>
-  </si>
-  <si>
-    <t>medium value</t>
-  </si>
-  <si>
-    <t>low value</t>
-  </si>
-  <si>
-    <t>very low value</t>
-  </si>
-  <si>
-    <t>rating_value</t>
+    <t>very high</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>medium</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>very low</t>
+  </si>
+  <si>
+    <t>rating_text</t>
+  </si>
+  <si>
+    <t>Super confusing, value versus impact…</t>
   </si>
 </sst>
 </file>
@@ -173,7 +176,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -200,9 +203,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -542,7 +542,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="44.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -563,6 +563,11 @@
         <v>7</v>
       </c>
     </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+    </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>13</v>
@@ -590,8 +595,8 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>8</v>
+      <c r="A7" t="s">
+        <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>0</v>
@@ -617,8 +622,8 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
-        <v>9</v>
+      <c r="A8" t="s">
+        <v>11</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="8">
@@ -642,7 +647,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="10" t="s">
+      <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="1"/>
@@ -667,8 +672,8 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="10" t="s">
-        <v>11</v>
+      <c r="A10" t="s">
+        <v>9</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="8">
@@ -692,8 +697,8 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
-        <v>12</v>
+      <c r="A11" t="s">
+        <v>8</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="9">
@@ -717,8 +722,8 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>8</v>
+      <c r="A12" t="s">
+        <v>12</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>1</v>
@@ -744,8 +749,8 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="10" t="s">
-        <v>9</v>
+      <c r="A13" t="s">
+        <v>11</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="8">
@@ -769,7 +774,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="10" t="s">
+      <c r="A14" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="1"/>
@@ -794,8 +799,8 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="10" t="s">
-        <v>11</v>
+      <c r="A15" t="s">
+        <v>9</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="8">
@@ -819,8 +824,8 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
-        <v>12</v>
+      <c r="A16" t="s">
+        <v>8</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="9">
@@ -844,8 +849,8 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>8</v>
+      <c r="A17" t="s">
+        <v>12</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>2</v>
@@ -871,8 +876,8 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="10" t="s">
-        <v>9</v>
+      <c r="A18" t="s">
+        <v>11</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="8">
@@ -896,7 +901,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="10" t="s">
+      <c r="A19" t="s">
         <v>10</v>
       </c>
       <c r="B19" s="1"/>
@@ -921,8 +926,8 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="10" t="s">
-        <v>11</v>
+      <c r="A20" t="s">
+        <v>9</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="8">
@@ -946,8 +951,8 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="5" t="s">
-        <v>12</v>
+      <c r="A21" t="s">
+        <v>8</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="9">
@@ -971,8 +976,8 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
-        <v>8</v>
+      <c r="A22" t="s">
+        <v>12</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>3</v>
@@ -998,8 +1003,8 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="10" t="s">
-        <v>9</v>
+      <c r="A23" t="s">
+        <v>11</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="8">
@@ -1023,7 +1028,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="10" t="s">
+      <c r="A24" t="s">
         <v>10</v>
       </c>
       <c r="B24" s="1"/>
@@ -1048,8 +1053,8 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="10" t="s">
-        <v>11</v>
+      <c r="A25" t="s">
+        <v>9</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="8">
@@ -1073,8 +1078,8 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="5" t="s">
-        <v>12</v>
+      <c r="A26" t="s">
+        <v>8</v>
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="9">

</xml_diff>